<commit_message>
data prep next steps
</commit_message>
<xml_diff>
--- a/rawdata/11_deferred_status_reclassification.xlsx
+++ b/rawdata/11_deferred_status_reclassification.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uzh-my.sharepoint.com/personal/elenamaria_goedde_uzh_ch/Documents/Desktop/Files for Coding/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chrstein\Documents\pwicloud_MyDrive\ECOSOC\ECOSOC_Status\rawdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="90" documentId="13_ncr:1_{84166DFC-FE2F-422A-A117-ABF3D8DEF4E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{68240E39-F8D9-491B-B85F-E2D92F95BAA4}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93D807C8-5747-4D94-99F9-B7AF83FFBEB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="910" yWindow="0" windowWidth="11780" windowHeight="11370" xr2:uid="{B9FD81F2-9F3E-4B5D-B02F-4CED1BF07905}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{B9FD81F2-9F3E-4B5D-B02F-4CED1BF07905}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="43">
   <si>
     <t>NGO_name</t>
   </si>
@@ -162,6 +162,9 @@
   </si>
   <si>
     <t>also mentioned  in: 13.07.2000</t>
+  </si>
+  <si>
+    <t>info</t>
   </si>
 </sst>
 </file>
@@ -226,14 +229,10 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 – 2022-Design">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 – 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -271,7 +270,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 – 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -377,7 +376,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 – 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -519,7 +518,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -529,8 +528,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8DF6FD1-8F94-4490-B5C8-A9EF3BC3EE11}">
   <dimension ref="A1:C67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" zoomScale="110" workbookViewId="0">
-      <selection activeCell="A70" sqref="A70"/>
+    <sheetView tabSelected="1" zoomScale="110" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -538,15 +537,18 @@
     <col min="1" max="1" width="42.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C1" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -554,7 +556,7 @@
         <v>45457</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -562,7 +564,7 @@
         <v>45457</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -570,7 +572,7 @@
         <v>43868</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -578,7 +580,7 @@
         <v>43868</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -586,7 +588,7 @@
         <v>43868</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -594,7 +596,7 @@
         <v>43620</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -602,7 +604,7 @@
         <v>43504</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -610,7 +612,7 @@
         <v>43504</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -618,7 +620,7 @@
         <v>43504</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -626,7 +628,7 @@
         <v>43154</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -634,7 +636,7 @@
         <v>43154</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -642,7 +644,7 @@
         <v>43154</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -650,7 +652,7 @@
         <v>43154</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>6</v>
       </c>
@@ -658,7 +660,7 @@
         <v>43154</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>12</v>
       </c>

</xml_diff>